<commit_message>
add unlock permanance script
</commit_message>
<xml_diff>
--- a/eKYC/api-ekyc/Counter_service.xlsx
+++ b/eKYC/api-ekyc/Counter_service.xlsx
@@ -516,7 +516,7 @@
   <dimension ref="A2:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -627,7 +627,7 @@
       </c>
       <c r="C3" s="11" t="inlineStr">
         <is>
-          <t>20220702-03</t>
+          <t>20220706-01</t>
         </is>
       </c>
       <c r="D3" s="15" t="inlineStr">
@@ -653,38 +653,38 @@
       </c>
       <c r="I3" s="8" t="inlineStr">
         <is>
-          <t>EQ2022070200010</t>
+          <t>-</t>
         </is>
       </c>
       <c r="J3" s="8" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2018</t>
         </is>
       </c>
       <c r="K3" s="8" t="inlineStr">
         <is>
-          <t>Success</t>
+          <t>QR match fail</t>
         </is>
       </c>
       <c r="L3" s="8" t="inlineStr"/>
       <c r="M3" s="8" t="inlineStr">
         <is>
-          <t>S0001</t>
+          <t>E0012</t>
         </is>
       </c>
       <c r="N3" s="8" t="inlineStr">
         <is>
-          <t>Success</t>
+          <t>The information of ID card and QR code is not matched.</t>
         </is>
       </c>
       <c r="O3" s="8" t="inlineStr">
         <is>
-          <t>ดำเนินการสำเร็จ</t>
+          <t>ข้อมูลบัตรประจำตัวประชาชนและ QR Code ไม่ตรงกัน</t>
         </is>
       </c>
       <c r="P3" s="18" t="inlineStr">
         <is>
-          <t>{"status":{"code":"0","message":"Success","remark":"","user_code":"S0001","user_message_en":"Success","user_message_th":"ดำเนินการสำเร็จ"},"data":{"journey_code":"JN003","journey_name":"EKYC QR Signup","kyc_trans_id":"EQ2022070200010"}}</t>
+          <t>{"status":{"code":"2018","message":"QR match fail","remark":"","user_code":"E0012","user_message_en":"The information of ID card and QR code is not matched.","user_message_th":"ข้อมูลบัตรประจำตัวประชาชนและ QR Code ไม่ตรงกัน"},"data":null}</t>
         </is>
       </c>
     </row>

</xml_diff>